<commit_message>
jenkins job config and started for lowmart
</commit_message>
<xml_diff>
--- a/src/test/resources/Documents/25904/Actual/JobMaterial.xlsx
+++ b/src/test/resources/Documents/25904/Actual/JobMaterial.xlsx
@@ -71,27 +71,27 @@
     <t>Ink / Varnish</t>
   </si>
   <si>
+    <t>Pantone-1 - UV</t>
+  </si>
+  <si>
+    <t>0.14</t>
+  </si>
+  <si>
+    <t>lbs</t>
+  </si>
+  <si>
+    <t>UV-PMS - UV-PMS</t>
+  </si>
+  <si>
     <t>Black - UV</t>
   </si>
   <si>
     <t>0.08</t>
   </si>
   <si>
-    <t>lbs</t>
-  </si>
-  <si>
     <t>UV-4 CP - UV- 4 Color Process</t>
   </si>
   <si>
-    <t>Pantone-1 - UV</t>
-  </si>
-  <si>
-    <t>0.14</t>
-  </si>
-  <si>
-    <t>UV-PMS - UV-PMS</t>
-  </si>
-  <si>
     <t>Print F (Varnish 1x0)</t>
   </si>
   <si>
@@ -107,6 +107,12 @@
     <t>Plate</t>
   </si>
   <si>
+    <t>Cyrel Plate</t>
+  </si>
+  <si>
+    <t>450 - ***40" Cyrel Plate for Press_________***</t>
+  </si>
+  <si>
     <t>Plate - Outer wrap  2p</t>
   </si>
   <si>
@@ -120,12 +126,6 @@
   </si>
   <si>
     <t>CTP40 - CTP Plate 40"</t>
-  </si>
-  <si>
-    <t>Cyrel Plate</t>
-  </si>
-  <si>
-    <t>450 - ***40" Cyrel Plate for Press_________***</t>
   </si>
   <si>
     <t>Sheet</t>
@@ -740,16 +740,16 @@
         <v>30</v>
       </c>
       <c r="B6" t="s" s="35">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s" s="36">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s" s="37">
         <v>31</v>
       </c>
-      <c r="C6" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s" s="37">
-        <v>33</v>
-      </c>
       <c r="E6" t="s" s="38">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s" s="39">
         <v>15</v>
@@ -758,7 +758,7 @@
         <v>16</v>
       </c>
       <c r="H6" t="s" s="41">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
@@ -766,16 +766,16 @@
         <v>30</v>
       </c>
       <c r="B7" t="s" s="43">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s" s="44">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s" s="45">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s" s="46">
         <v>36</v>
-      </c>
-      <c r="E7" t="s" s="46">
-        <v>14</v>
       </c>
       <c r="F7" t="s" s="47">
         <v>15</v>

</xml_diff>